<commit_message>
bugfix: source file revenue numbers
</commit_message>
<xml_diff>
--- a/source/a_revenue_report_23_2025_09.xlsx
+++ b/source/a_revenue_report_23_2025_09.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -146,19 +146,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="128"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="128"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="128"/>
     </font>
     <font>
       <sz val="11"/>
@@ -263,7 +260,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -290,6 +287,10 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -369,112 +370,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -483,7 +378,7 @@
   <dimension ref="A1:W559"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55859375" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -529,22 +424,22 @@
       <c r="W1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="2" t="n">
         <v>3522.67844</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="2" t="n">
         <v>1445.61886</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="2" t="n">
         <v>820.062793</v>
       </c>
       <c r="G2" s="1" t="n">
@@ -560,22 +455,22 @@
       <c r="O2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="n">
         <v>0.045281</v>
       </c>
       <c r="G3" s="1" t="n">
@@ -584,22 +479,22 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="2" t="n">
         <v>149.066543</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="2" t="n">
         <v>83.44385</v>
       </c>
       <c r="G4" s="1" t="n">
@@ -608,22 +503,22 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="2" t="n">
         <v>0.679995</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="2" t="n">
         <v>0.492044</v>
       </c>
       <c r="G5" s="1" t="n">
@@ -632,22 +527,22 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="2" t="n">
         <v>237.590008</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="2" t="n">
         <v>239.919255</v>
       </c>
       <c r="G6" s="1" t="n">
@@ -655,47 +550,46 @@
         <v>477.509263</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="2" t="n">
         <v>18.561558</v>
       </c>
-      <c r="F7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <f aca="false">SUM(D7:F7)</f>
-        <v>18.561558</v>
+      <c r="F7" s="7" t="n">
+        <v>6.7551</v>
+      </c>
+      <c r="G7" s="7" t="n">
+        <v>25.316658</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="2" t="n">
         <v>181.582799</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="2" t="n">
         <v>147.684362</v>
       </c>
       <c r="G8" s="1" t="n">
@@ -704,22 +598,22 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="2" t="n">
         <v>90.566203</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="2" t="n">
         <v>64.316896</v>
       </c>
       <c r="G9" s="1" t="n">
@@ -728,22 +622,22 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="2" t="n">
         <v>20625.519089</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="2" t="n">
         <v>15576.680221</v>
       </c>
       <c r="G10" s="1" t="n">

</xml_diff>